<commit_message>
Add further tests for NetworkCost class. Reorganize modules. Rework classes to proximately transfer responsibilities to FreightNetwork class.
</commit_message>
<xml_diff>
--- a/components/test_data/test_railway_parameters.xlsx
+++ b/components/test_data/test_railway_parameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="mob" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="79">
   <si>
     <t>turnout_freq</t>
   </si>
@@ -244,6 +244,18 @@
   </si>
   <si>
     <t>yearly_wages_by_turnout</t>
+  </si>
+  <si>
+    <t>net_to_gross_factor</t>
+  </si>
+  <si>
+    <t>Factor to convert (aproximately) net tons to gross tons, based on a full train operation (coef).</t>
+  </si>
+  <si>
+    <t>main_min_density</t>
+  </si>
+  <si>
+    <t>Minimum density to consider a link as being a main track (ton-km/ton = ton).</t>
   </si>
 </sst>
 </file>
@@ -620,10 +632,10 @@
     <tabColor theme="7" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,6 +882,28 @@
       </c>
       <c r="C22" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" s="4">
+        <v>1.67</v>
+      </c>
+      <c r="C23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="5">
+        <v>760000</v>
+      </c>
+      <c r="C24" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -885,7 +919,7 @@
   </sheetPr>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>

</xml_diff>